<commit_message>
generate prism data for peak count
</commit_message>
<xml_diff>
--- a/data/230608-prism-peak-counts-output.xlsx
+++ b/data/230608-prism-peak-counts-output.xlsx
@@ -364,6 +364,156 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -389,6 +539,156 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>